<commit_message>
Pathways per gene Excel file | Probe correction extension | tests
</commit_message>
<xml_diff>
--- a/examples/my_folder_name_with_extension/genes_per_cell.xlsx
+++ b/examples/my_folder_name_with_extension/genes_per_cell.xlsx
@@ -169,16 +169,16 @@
     <t>Fos, Jun</t>
   </si>
   <si>
-    <t>COX1, COX2, COX3, Cox4i1, Cox4i2, Cox5a, Cox5b, Cox6a1, Cox6a2, Cox6b1, Cox6b2, Cox6c, Cox7a1, Cox7a2, Cox7a2l, Cox7b, Cox7b2, Cox7c, Cox8a, Cox8b, Cox8c</t>
-  </si>
-  <si>
-    <t>Ndufa1, Ndufa10, Ndufa11, Ndufa12, Ndufa13, Ndufa2, Ndufa3, Ndufa4, Ndufa4l2, Ndufa5, Ndufa6, Ndufa7, Ndufa8, Ndufa9, Ndufab1, Ndufb1, Ndufb10, Ndufb11, Ndufb2, Ndufb3, Ndufb4, Ndufb4b, Ndufb4c, Ndufb5, Ndufb6, Ndufb7, Ndufb8, Ndufb9, Ndufc1, Ndufc2, Ndufs1, Ndufs2, Ndufs3, Ndufs4, Ndufs5, Ndufs6, Ndufs7, Ndufs8, Ndufv1, Ndufv2, Ndufv3</t>
+    <t>COX1, COX2, COX3, Cox4i1, Cox4i2, Cox5a, Cox5b, Cox6a1, Cox6a2, Cox6b1, Cox6b2, Cox6c, Cox7a1, Cox7a2, Cox7a2l, Cox7b, Cox7b2, Cox7c, Cox8a, Cox8b, Cox8c, Gm11633</t>
+  </si>
+  <si>
+    <t>Gm19340, Ndufa1, Ndufa10, Ndufa11, Ndufa12, Ndufa13, Ndufa2, Ndufa3, Ndufa4, Ndufa4l2, Ndufa5, Ndufa6, Ndufa7, Ndufa8, Ndufa9, Ndufab1, Ndufab1-ps, Ndufb1, Ndufb10, Ndufb11, Ndufb2, Ndufb3, Ndufb4, Ndufb4b, Ndufb4c, Ndufb5, Ndufb6, Ndufb7, Ndufb8, Ndufb9, Ndufc1, Ndufc2, Ndufs1, Ndufs2, Ndufs3, Ndufs4, Ndufs5, Ndufs6, Ndufs7, Ndufs8, Ndufv1, Ndufv2, Ndufv3</t>
   </si>
   <si>
     <t>Sdha, Sdhb, Sdhc, Sdhd</t>
   </si>
   <si>
-    <t>CYTB, Cyc1, Uqcr10, Uqcr11, Uqcrb, Uqcrc1, Uqcrc2, Uqcrfs1, Uqcrh, Uqcrq</t>
+    <t>CYTB, Cyc1, Gm6293, Uqcr10, Uqcr11, Uqcrb, Uqcrc1, Uqcrc2, Uqcrfs1, Uqcrh, Uqcrq</t>
   </si>
   <si>
     <t>Mapk11, Mapk12, Mapk13, Mapk14</t>

</xml_diff>